<commit_message>
change the background picture
</commit_message>
<xml_diff>
--- a/miscellaneous/internships.jobs/internships_edited.xlsx
+++ b/miscellaneous/internships.jobs/internships_edited.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="466">
   <si>
     <t>Deadline</t>
   </si>
@@ -1492,12 +1492,15 @@
   <si>
     <t>Zinzi Blackbeard</t>
   </si>
+  <si>
+    <t>two</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1574,6 +1577,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1602,7 +1612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1632,6 +1642,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2023,8 +2034,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G263"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="G150" sqref="G150"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,8 +5383,8 @@
       <c r="B148" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C148" s="6">
-        <v>81</v>
+      <c r="C148" s="6" t="s">
+        <v>465</v>
       </c>
       <c r="D148" s="6">
         <v>14000</v>
@@ -6643,7 +6654,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId148" name="Control 6">
+        <control shapeId="1029" r:id="rId148" name="Control 5">
           <controlPr defaultSize="0" r:id="rId149">
             <anchor moveWithCells="1">
               <from>
@@ -6663,12 +6674,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId148" name="Control 6"/>
+        <control shapeId="1029" r:id="rId148" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId150" name="Control 5">
+        <control shapeId="1030" r:id="rId150" name="Control 6">
           <controlPr defaultSize="0" r:id="rId149">
             <anchor moveWithCells="1">
               <from>
@@ -6688,7 +6699,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId150" name="Control 5"/>
+        <control shapeId="1030" r:id="rId150" name="Control 6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6699,8 +6710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6749,8 +6760,8 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>219</v>
       </c>
     </row>

</xml_diff>